<commit_message>
Refactored code and fixed value in test file.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dusty/Desktop/excel_script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dusty/Desktop/PartMirror/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FE42B7-F069-E949-A2D7-10972E1C60E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875605D-1BE9-9542-801F-57A51484C669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="2960" windowWidth="27240" windowHeight="16440" xr2:uid="{55D7C136-13CB-5E4E-9D25-ABA659EA8D62}"/>
   </bookViews>
@@ -255,9 +255,6 @@
     <t>Х5 Е70</t>
   </si>
   <si>
-    <t>X5 E70, X6 E71, C-Max, C216, W221, Espace 4, Grand Scenic 2, Koleos, Laguna 2, Laguna 3, Scenic 2, Vel Satis</t>
-  </si>
-  <si>
     <t>8pin</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Цвет</t>
+  </si>
+  <si>
+    <t>X5 E70, X6 E71, C-Max, C216, W221, Espace 4, Grand Scenic, Koleos, Laguna 2, Laguna 3, Scenic 2, Vel Satis</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A863D6ED-509D-6640-A7A6-DA6654A0E805}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,31 +745,31 @@
         <v>15</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>16</v>
@@ -841,19 +841,19 @@
         <v>38</v>
       </c>
       <c r="AV1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="AZ1" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -970,12 +970,12 @@
         <v>63</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
       <c r="AT2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>

</xml_diff>

<commit_message>
Updated processing of cyrillic values in mirrors.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dusty/Desktop/PartMirror/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dusty/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875605D-1BE9-9542-801F-57A51484C669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9823AA-609E-8144-8FCB-05FD65D74BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="2960" windowWidth="27240" windowHeight="16440" xr2:uid="{55D7C136-13CB-5E4E-9D25-ABA659EA8D62}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>

</xml_diff>